<commit_message>
Updated report's forms:  - added new form;  - updated report template;  - updated one form;  - added new parameters.
</commit_message>
<xml_diff>
--- a/Parameters/BProg.xlsx
+++ b/Parameters/BProg.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DES.LM.Reports\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D55B15E-797C-46BB-A118-DECFAE13B651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA12C40-4C96-4942-A4D9-BBA55581537A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2730" windowWidth="29040" windowHeight="15840" xr2:uid="{184954BB-DCC8-4745-A6E6-04D458187FA2}"/>
+    <workbookView xWindow="-28920" yWindow="-12045" windowWidth="29040" windowHeight="17640" xr2:uid="{184954BB-DCC8-4745-A6E6-04D458187FA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>ID_DES.LM_project</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t>Full_Project_name</t>
+  </si>
+  <si>
+    <t>IS_Service_type</t>
+  </si>
+  <si>
+    <t>IS_Product_type</t>
   </si>
 </sst>
 </file>
@@ -117,9 +123,10 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -438,21 +445,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3F2C30A-8E50-404E-92D3-C8D178933546}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -460,11 +469,17 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{A3F2C30A-8E50-404E-92D3-C8D178933546}"/>
+  <autoFilter ref="A1:E1" xr:uid="{A3F2C30A-8E50-404E-92D3-C8D178933546}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>